<commit_message>
add iycf_quality_report and small fixes
</commit_message>
<xml_diff>
--- a/inst/iycf_quality_report/resources/overall_plaus.xlsx
+++ b/inst/iycf_quality_report/resources/overall_plaus.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abraham.azar\Desktop\git\impactR4PHU\inst\fsl_quality_report\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abraham.azar\Desktop\git\impactR4PHU\inst\iycf_quality_report\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D0C352-CB79-4A6A-9094-765C5F0C6B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E16817E-F9BA-4DF8-AB0B-EF8C84B54229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FSL" sheetId="1" r:id="rId1"/>
     <sheet name="NUT" sheetId="2" r:id="rId2"/>
     <sheet name="MORT" sheetId="3" r:id="rId3"/>
+    <sheet name="IYCF" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="129">
   <si>
     <t>flag_name</t>
   </si>
@@ -356,6 +357,75 @@
   </si>
   <si>
     <t>&gt;= 30</t>
+  </si>
+  <si>
+    <t>plaus_sdd_mdd</t>
+  </si>
+  <si>
+    <t>plaus_age_ratio_under6m_6to23m.pvalue</t>
+  </si>
+  <si>
+    <t>plaus_prop_flag_high_mdd_low_mmf</t>
+  </si>
+  <si>
+    <t>plaus_mad_ratio.pvalue</t>
+  </si>
+  <si>
+    <t>plaus_prop_iycf_caregiver</t>
+  </si>
+  <si>
+    <t>&gt;=0.9</t>
+  </si>
+  <si>
+    <t>&gt;=0.8</t>
+  </si>
+  <si>
+    <t>&gt;=0.7</t>
+  </si>
+  <si>
+    <t>&gt;=0.5</t>
+  </si>
+  <si>
+    <t>&lt;0.01</t>
+  </si>
+  <si>
+    <t>&lt;0.05</t>
+  </si>
+  <si>
+    <t>&lt;0.1</t>
+  </si>
+  <si>
+    <t>&gt;=0.1</t>
+  </si>
+  <si>
+    <t>&lt;=0.001</t>
+  </si>
+  <si>
+    <t>&gt; 0.0001</t>
+  </si>
+  <si>
+    <t>&gt;0.01</t>
+  </si>
+  <si>
+    <t>plaus_iycf_score</t>
+  </si>
+  <si>
+    <t>plaus_iycf_cat</t>
+  </si>
+  <si>
+    <t>10 &lt; 15</t>
+  </si>
+  <si>
+    <t>15 &lt; 25</t>
+  </si>
+  <si>
+    <t>&gt;1 &amp; &lt;2</t>
+  </si>
+  <si>
+    <t>&gt;0.8 &amp; &lt;2.2</t>
+  </si>
+  <si>
+    <t>&lt;=0.8 or &gt;=2.2</t>
   </si>
 </sst>
 </file>
@@ -423,7 +493,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -747,11 +817,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -950,6 +1072,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1233,8 +1367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2586,7 +2720,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection sqref="A1:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2848,4 +2982,265 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0CF2A9B-F33F-4227-A567-5035D9106014}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="15"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="65" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="67" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="68"/>
+      <c r="E2" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="64"/>
+      <c r="B3" s="20">
+        <v>0</v>
+      </c>
+      <c r="C3" s="69">
+        <v>5</v>
+      </c>
+      <c r="D3" s="70"/>
+      <c r="E3" s="21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="66"/>
+      <c r="B5" s="20">
+        <v>0</v>
+      </c>
+      <c r="C5" s="20">
+        <v>2</v>
+      </c>
+      <c r="D5" s="20">
+        <v>5</v>
+      </c>
+      <c r="E5" s="21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="64"/>
+      <c r="B7" s="20">
+        <v>0</v>
+      </c>
+      <c r="C7" s="20">
+        <v>2</v>
+      </c>
+      <c r="D7" s="20">
+        <v>4</v>
+      </c>
+      <c r="E7" s="21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="63" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="64"/>
+      <c r="B9" s="20">
+        <v>0</v>
+      </c>
+      <c r="C9" s="20">
+        <v>5</v>
+      </c>
+      <c r="D9" s="20">
+        <v>10</v>
+      </c>
+      <c r="E9" s="21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="64"/>
+      <c r="B11" s="20">
+        <v>0</v>
+      </c>
+      <c r="C11" s="20">
+        <v>5</v>
+      </c>
+      <c r="D11" s="20">
+        <v>10</v>
+      </c>
+      <c r="E11" s="21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="64"/>
+      <c r="B13" s="20">
+        <v>0</v>
+      </c>
+      <c r="C13" s="20">
+        <v>2</v>
+      </c>
+      <c r="D13" s="20">
+        <v>5</v>
+      </c>
+      <c r="E13" s="21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>